<commit_message>
Adactin App changes 02-11-2022
</commit_message>
<xml_diff>
--- a/MavenFeb/Folder/TestData.xlsx
+++ b/MavenFeb/Folder/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\navee\OneDrive\Desktop\MavenFeb\Folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\New folder\New folder\New folder\Greens_NewEclipse_Sep20-2022\MavenFeb\Folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25BFEAC-8008-46FC-8D31-ECB2BBAC6827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA9027F-2324-41C1-B4D8-0471FA12B6FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{166FEB90-D0F5-479A-B9D2-CFB31B066EED}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{166FEB90-D0F5-479A-B9D2-CFB31B066EED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="54">
   <si>
     <t>SNO</t>
   </si>
@@ -88,9 +88,6 @@
     <t>Facebook helps you connect and share with the people in your life.</t>
   </si>
   <si>
-    <t>Adactin@123</t>
-  </si>
-  <si>
     <t>FirstName</t>
   </si>
   <si>
@@ -181,9 +178,6 @@
     <t>Adactin@130</t>
   </si>
   <si>
-    <t>NAVEENREDMINOTE10</t>
-  </si>
-  <si>
     <t>NAVEENREDMINOTE11</t>
   </si>
   <si>
@@ -203,14 +197,16 @@
   </si>
   <si>
     <t>NAVEENREDMINOTE17</t>
+  </si>
+  <si>
+    <t>NaveenSelenium</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -650,9 +646,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="70.6640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.33203125" collapsed="true"/>
+    <col min="3" max="3" width="70.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -759,11 +755,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId16" xr:uid="{18D887C2-2C48-4CBF-9F58-DED21E3F727C}"/>
-    <hyperlink ref="C3" r:id="rId17" xr:uid="{029C4400-1881-4EEE-ABCC-6753431F696D}"/>
-    <hyperlink ref="C4" r:id="rId18" xr:uid="{ACBD4621-885C-4D02-B802-0E91C83BA1CD}"/>
-    <hyperlink ref="C5" r:id="rId19" xr:uid="{1CDFF833-05AD-4B37-A488-E73AC7E112E9}"/>
-    <hyperlink ref="C6" r:id="rId20" xr:uid="{0846AC57-892A-49B7-A2DE-0A99E79559FB}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{18D887C2-2C48-4CBF-9F58-DED21E3F727C}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{029C4400-1881-4EEE-ABCC-6753431F696D}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{ACBD4621-885C-4D02-B802-0E91C83BA1CD}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{1CDFF833-05AD-4B37-A488-E73AC7E112E9}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{0846AC57-892A-49B7-A2DE-0A99E79559FB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -834,15 +830,15 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" customWidth="true" width="21.6640625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="26.6640625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="16.5546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="21.88671875" collapsed="true"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="26.6640625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.5546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="21.88671875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -850,25 +846,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>22</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -876,13 +872,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>26</v>
       </c>
       <c r="E2" s="6">
         <v>1234567891234560</v>
@@ -890,11 +886,11 @@
       <c r="F2" s="6">
         <v>123</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>16</v>
+      <c r="G2" s="8">
+        <v>123456</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -902,13 +898,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>29</v>
       </c>
       <c r="E3" s="6">
         <v>1234567890123450</v>
@@ -917,10 +913,10 @@
         <v>456</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -928,13 +924,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="E4" s="6">
         <v>1234567890123450</v>
@@ -943,10 +939,10 @@
         <v>789</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -954,13 +950,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>26</v>
       </c>
       <c r="E5" s="6">
         <v>1234567890123450</v>
@@ -969,10 +965,10 @@
         <v>123</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -980,13 +976,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>38</v>
-      </c>
       <c r="D6" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" s="6">
         <v>1234567890123450</v>
@@ -995,10 +991,10 @@
         <v>456</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -1006,13 +1002,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" s="6">
         <v>1234567890123450</v>
@@ -1021,10 +1017,10 @@
         <v>789</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -1032,13 +1028,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E8" s="6">
         <v>1234567890123450</v>
@@ -1047,10 +1043,10 @@
         <v>987</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -1058,13 +1054,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="D9" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" s="6">
         <v>1234567890123450</v>
@@ -1073,23 +1069,22 @@
         <v>678</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId25" xr:uid="{DDE3F650-C107-4ABC-B913-6CCB41053EED}"/>
-    <hyperlink ref="G3" r:id="rId26" display="Adactin@123" xr:uid="{F0764462-B15A-47D9-8231-F89B0D3B0A93}"/>
-    <hyperlink ref="G4" r:id="rId27" display="Adactin@123" xr:uid="{E90C57EF-32CC-4F26-A3B6-EDC1837D9978}"/>
-    <hyperlink ref="G5" r:id="rId28" display="Adactin@123" xr:uid="{F158E298-2E56-4693-B6D3-B822DB2BBDC7}"/>
-    <hyperlink ref="G6" r:id="rId29" display="Adactin@123" xr:uid="{CE14C63A-9862-48EF-A8C9-684D290AEB41}"/>
-    <hyperlink ref="G7" r:id="rId30" display="Adactin@123" xr:uid="{36C90806-D0FC-4794-8D45-0390010CFC73}"/>
-    <hyperlink ref="G8" r:id="rId31" display="Adactin@123" xr:uid="{CBFA6C27-A1BA-4981-8305-5F43AE9C135D}"/>
-    <hyperlink ref="G9" r:id="rId32" display="Adactin@123" xr:uid="{11C2E55C-9812-4026-A370-8E489F477E16}"/>
+    <hyperlink ref="G3" r:id="rId1" display="Adactin@123" xr:uid="{F0764462-B15A-47D9-8231-F89B0D3B0A93}"/>
+    <hyperlink ref="G4" r:id="rId2" display="Adactin@123" xr:uid="{E90C57EF-32CC-4F26-A3B6-EDC1837D9978}"/>
+    <hyperlink ref="G5" r:id="rId3" display="Adactin@123" xr:uid="{F158E298-2E56-4693-B6D3-B822DB2BBDC7}"/>
+    <hyperlink ref="G6" r:id="rId4" display="Adactin@123" xr:uid="{CE14C63A-9862-48EF-A8C9-684D290AEB41}"/>
+    <hyperlink ref="G7" r:id="rId5" display="Adactin@123" xr:uid="{36C90806-D0FC-4794-8D45-0390010CFC73}"/>
+    <hyperlink ref="G8" r:id="rId6" display="Adactin@123" xr:uid="{CBFA6C27-A1BA-4981-8305-5F43AE9C135D}"/>
+    <hyperlink ref="G9" r:id="rId7" display="Adactin@123" xr:uid="{11C2E55C-9812-4026-A370-8E489F477E16}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>